<commit_message>
Add audit files to data library
</commit_message>
<xml_diff>
--- a/Resources/Data Sets/JASP Examples Description.xlsx
+++ b/Resources/Data Sets/JASP Examples Description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jill/Jasp/jasp-desktop/Resources/Data Sets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JASP\jasp-desktop\Resources\Data Sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CC15F4F-708F-9B4C-B302-138B5A6A60A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F3B8DB-B245-4652-B786-732787AE8C66}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="84" yWindow="456" windowWidth="25440" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JASP Examples Description" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="224">
   <si>
     <t>Part</t>
   </si>
@@ -677,6 +677,21 @@
   </si>
   <si>
     <t>inspecting data thoroughly using plots rather than statistical output</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>BuildIt Binary</t>
+  </si>
+  <si>
+    <t>BuildIt Monetary</t>
+  </si>
+  <si>
+    <t>BuildIt's monetary audit population consisting of 3500 transactions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildIt's non-monetary audit population consisting of 3500 records. </t>
   </si>
 </sst>
 </file>
@@ -1517,25 +1532,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="56.19921875" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" customWidth="1"/>
+    <col min="7" max="7" width="28.296875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="25.69921875" customWidth="1"/>
     <col min="10" max="10" width="58.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1599,7 +1615,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +1647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1663,7 +1679,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1695,7 +1711,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1727,7 +1743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1759,7 +1775,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1791,7 +1807,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1817,7 +1833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1849,7 +1865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1881,7 +1897,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1913,7 +1929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1945,7 +1961,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1977,7 +1993,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2009,7 +2025,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -2041,7 +2057,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2073,7 +2089,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2105,7 +2121,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2137,7 +2153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -2169,7 +2185,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2201,7 +2217,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2233,7 +2249,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2265,7 +2281,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -2297,7 +2313,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -2329,7 +2345,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -2361,7 +2377,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -2393,7 +2409,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -2425,7 +2441,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -2457,7 +2473,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2489,7 +2505,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -2521,7 +2537,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2553,7 +2569,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2585,7 +2601,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -2617,7 +2633,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>125</v>
       </c>
@@ -2649,7 +2665,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -2681,7 +2697,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>125</v>
       </c>
@@ -2713,7 +2729,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -2745,7 +2761,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -2777,7 +2793,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>125</v>
       </c>
@@ -2809,7 +2825,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -2841,7 +2857,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -2873,7 +2889,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -2905,7 +2921,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -2937,7 +2953,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -2969,7 +2985,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -3001,7 +3017,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>173</v>
       </c>
@@ -3033,7 +3049,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>179</v>
       </c>
@@ -3065,7 +3081,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>184</v>
       </c>
@@ -3097,71 +3113,47 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>188</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>189</v>
-      </c>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>13</v>
       </c>
       <c r="E50" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="F50" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="G50" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="H50" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="I50" t="s">
         <v>13</v>
       </c>
-      <c r="J50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>188</v>
-      </c>
-      <c r="B51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" t="s">
-        <v>193</v>
-      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="F51" t="s">
-        <v>92</v>
+        <v>219</v>
       </c>
       <c r="G51" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="H51" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="I51" t="s">
         <v>13</v>
       </c>
-      <c r="J51" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>188</v>
       </c>
@@ -3169,62 +3161,127 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
+        <v>189</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
+        <v>190</v>
+      </c>
+      <c r="F52" t="s">
+        <v>191</v>
+      </c>
+      <c r="G52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H52" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="s">
+        <v>194</v>
+      </c>
+      <c r="F53" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" t="s">
+        <v>195</v>
+      </c>
+      <c r="H53" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
         <v>197</v>
       </c>
-      <c r="D52" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" t="s">
         <v>198</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G54" t="s">
         <v>199</v>
       </c>
-      <c r="H52" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="H54" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>200</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>201</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>202</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F56" t="s">
         <v>203</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H56" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>205</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>206</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>207</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>202</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G57" t="s">
         <v>208</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I57" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add audit files to data library (#3365)
</commit_message>
<xml_diff>
--- a/Resources/Data Sets/JASP Examples Description.xlsx
+++ b/Resources/Data Sets/JASP Examples Description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jill/Jasp/jasp-desktop/Resources/Data Sets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JASP\jasp-desktop\Resources\Data Sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CC15F4F-708F-9B4C-B302-138B5A6A60A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F3B8DB-B245-4652-B786-732787AE8C66}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="84" yWindow="456" windowWidth="25440" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JASP Examples Description" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="224">
   <si>
     <t>Part</t>
   </si>
@@ -677,6 +677,21 @@
   </si>
   <si>
     <t>inspecting data thoroughly using plots rather than statistical output</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>BuildIt Binary</t>
+  </si>
+  <si>
+    <t>BuildIt Monetary</t>
+  </si>
+  <si>
+    <t>BuildIt's monetary audit population consisting of 3500 transactions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildIt's non-monetary audit population consisting of 3500 records. </t>
   </si>
 </sst>
 </file>
@@ -1517,25 +1532,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="56.19921875" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" customWidth="1"/>
+    <col min="7" max="7" width="28.296875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="25.69921875" customWidth="1"/>
     <col min="10" max="10" width="58.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1599,7 +1615,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +1647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1663,7 +1679,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1695,7 +1711,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1727,7 +1743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1759,7 +1775,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1791,7 +1807,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1817,7 +1833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1849,7 +1865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1881,7 +1897,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1913,7 +1929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1945,7 +1961,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1977,7 +1993,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2009,7 +2025,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -2041,7 +2057,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2073,7 +2089,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2105,7 +2121,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2137,7 +2153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -2169,7 +2185,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2201,7 +2217,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2233,7 +2249,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2265,7 +2281,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -2297,7 +2313,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -2329,7 +2345,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -2361,7 +2377,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -2393,7 +2409,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -2425,7 +2441,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -2457,7 +2473,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2489,7 +2505,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -2521,7 +2537,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2553,7 +2569,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2585,7 +2601,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -2617,7 +2633,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>125</v>
       </c>
@@ -2649,7 +2665,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -2681,7 +2697,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>125</v>
       </c>
@@ -2713,7 +2729,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -2745,7 +2761,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -2777,7 +2793,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>125</v>
       </c>
@@ -2809,7 +2825,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -2841,7 +2857,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -2873,7 +2889,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -2905,7 +2921,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -2937,7 +2953,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -2969,7 +2985,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -3001,7 +3017,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>173</v>
       </c>
@@ -3033,7 +3049,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>179</v>
       </c>
@@ -3065,7 +3081,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>184</v>
       </c>
@@ -3097,71 +3113,47 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>188</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>189</v>
-      </c>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>13</v>
       </c>
       <c r="E50" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="F50" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="G50" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="H50" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="I50" t="s">
         <v>13</v>
       </c>
-      <c r="J50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>188</v>
-      </c>
-      <c r="B51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" t="s">
-        <v>193</v>
-      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="F51" t="s">
-        <v>92</v>
+        <v>219</v>
       </c>
       <c r="G51" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="H51" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="I51" t="s">
         <v>13</v>
       </c>
-      <c r="J51" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>188</v>
       </c>
@@ -3169,62 +3161,127 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
+        <v>189</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
+        <v>190</v>
+      </c>
+      <c r="F52" t="s">
+        <v>191</v>
+      </c>
+      <c r="G52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H52" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="s">
+        <v>194</v>
+      </c>
+      <c r="F53" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" t="s">
+        <v>195</v>
+      </c>
+      <c r="H53" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
         <v>197</v>
       </c>
-      <c r="D52" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" t="s">
         <v>198</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G54" t="s">
         <v>199</v>
       </c>
-      <c r="H52" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="H54" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>200</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>201</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>202</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F56" t="s">
         <v>203</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H56" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>205</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>206</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>207</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>202</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G57" t="s">
         <v>208</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I57" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>